<commit_message>
Fixes and prep for distribution on different hosted notebook providers
</commit_message>
<xml_diff>
--- a/Week 1/Week 1 Challenge.xlsx
+++ b/Week 1/Week 1 Challenge.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Logistic Regression" sheetId="2" r:id="rId2"/>
-    <sheet name="1 Layer Wine Net" sheetId="3" r:id="rId3"/>
+    <sheet name="2 Layer Wine Net" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -358,10 +358,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -682,42 +682,42 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:34" ht="37" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="P1" s="12" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="V1" s="12" t="s">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="V1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -20050,7 +20050,7 @@
   <dimension ref="A1:BD180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BD3" sqref="BD3"/>
+      <selection activeCell="AD2" sqref="AD2:AF180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31502,8 +31502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CU180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CG1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="CU3" sqref="CU3"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31711,7 +31711,7 @@
       <c r="AL3" s="3"/>
       <c r="AM3" s="4"/>
       <c r="AN3" s="1"/>
-      <c r="AO3" s="13"/>
+      <c r="AO3" s="12"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="2"/>
       <c r="AR3" s="3"/>

</xml_diff>